<commit_message>
updated pops files, etc
</commit_message>
<xml_diff>
--- a/data/coho_coastw_pops_TABLE.xlsx
+++ b/data/coho_coastw_pops_TABLE.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26929"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="8200" yWindow="0" windowWidth="41320" windowHeight="27120" tabRatio="500"/>
+    <workbookView xWindow="6640" yWindow="1200" windowWidth="41320" windowHeight="27120" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="digest table 2003 &amp; 2015 sampl" sheetId="4" r:id="rId1"/>
@@ -45,7 +45,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-order may need to be adjusted slightly, pending lat-long coordinates</t>
+order may need to be adjusted slightly, pending lat-long coordinates; currently based on approximate lat longs, not actual ones 042816</t>
         </r>
       </text>
     </comment>
@@ -172,6 +172,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t>Libby Gilbert-Horvath:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+pending receipt of actual GPS coords for each sample site from collaborators 042816</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F2" authorId="0">
       <text>
         <r>
@@ -196,7 +220,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F4" authorId="0">
+    <comment ref="F6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -220,7 +244,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F6" authorId="0">
+    <comment ref="F9" authorId="0">
       <text>
         <r>
           <rPr>
@@ -541,7 +565,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="564" uniqueCount="284">
   <si>
     <t>14</t>
     <phoneticPr fontId="0" type="noConversion"/>
@@ -1436,12 +1460,45 @@
   <si>
     <t>20 and 25</t>
   </si>
+  <si>
+    <t>42.740624, -124.395111</t>
+  </si>
+  <si>
+    <t>Very approx Lat Long (Google Maps)</t>
+  </si>
+  <si>
+    <t>not found</t>
+  </si>
+  <si>
+    <t>42.470447, -124.385725</t>
+  </si>
+  <si>
+    <t>42.402343, -123.921119</t>
+  </si>
+  <si>
+    <t>42.368323, -123.549802</t>
+  </si>
+  <si>
+    <t>42.442224, -123.683924</t>
+  </si>
+  <si>
+    <t>42.703322, -122.740267</t>
+  </si>
+  <si>
+    <t>42.655645, -123.061591</t>
+  </si>
+  <si>
+    <t>42.117040, -124.181852</t>
+  </si>
+  <si>
+    <t>42.055376, -124.211247</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1574,6 +1631,17 @@
       <color theme="9" tint="-0.499984740745262"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF999999"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF4285F4"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -1742,7 +1810,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1858,6 +1926,8 @@
     <xf numFmtId="0" fontId="7" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="127">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -2315,15 +2385,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N48"/>
+  <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="D48" sqref="D48"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" customWidth="1"/>
+    <col min="1" max="1" width="7.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.28515625" customWidth="1"/>
     <col min="3" max="3" width="15" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
@@ -2333,13 +2403,13 @@
     <col min="8" max="8" width="14" customWidth="1"/>
     <col min="9" max="9" width="9.5703125" customWidth="1"/>
     <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="33.28515625" customWidth="1"/>
-    <col min="12" max="12" width="8.85546875" customWidth="1"/>
-    <col min="13" max="13" width="6.7109375" customWidth="1"/>
-    <col min="14" max="14" width="52.140625" customWidth="1"/>
+    <col min="11" max="12" width="33.28515625" customWidth="1"/>
+    <col min="13" max="13" width="8.85546875" customWidth="1"/>
+    <col min="14" max="14" width="6.7109375" customWidth="1"/>
+    <col min="15" max="15" width="52.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="28" customFormat="1" ht="52" customHeight="1">
+    <row r="1" spans="1:15" s="28" customFormat="1" ht="52" customHeight="1">
       <c r="A1" s="29" t="s">
         <v>206</v>
       </c>
@@ -2373,18 +2443,21 @@
       <c r="K1" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="14" t="s">
+      <c r="L1" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="M1" s="14" t="s">
         <v>145</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="N1" s="14" t="s">
         <v>148</v>
       </c>
-      <c r="N1" s="14" t="s">
+      <c r="O1" s="14" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="22" customFormat="1">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:15" s="22" customFormat="1">
+      <c r="A2" s="1" t="s">
         <v>207</v>
       </c>
       <c r="B2" s="13" t="s">
@@ -2417,18 +2490,21 @@
       <c r="K2" s="11" t="s">
         <v>153</v>
       </c>
-      <c r="L2" s="1" t="s">
+      <c r="L2" s="53" t="s">
+        <v>273</v>
+      </c>
+      <c r="M2" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="N2" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="O2" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="22" customFormat="1">
-      <c r="A3" s="22" t="s">
+    <row r="3" spans="1:15" s="22" customFormat="1">
+      <c r="A3" s="1" t="s">
         <v>208</v>
       </c>
       <c r="B3" s="13" t="s">
@@ -2461,34 +2537,37 @@
       <c r="K3" s="11" t="s">
         <v>152</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="L3" s="11" t="s">
+        <v>275</v>
+      </c>
+      <c r="M3" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="22" customFormat="1">
+    <row r="4" spans="1:15" s="22" customFormat="1">
       <c r="A4" s="22" t="s">
         <v>209</v>
       </c>
-      <c r="B4" s="13" t="s">
-        <v>157</v>
+      <c r="B4" s="24" t="s">
+        <v>167</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D4" s="34" t="s">
+      <c r="D4" s="37" t="s">
         <v>60</v>
       </c>
       <c r="E4" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>189</v>
-      </c>
-      <c r="G4" s="42">
-        <v>1</v>
+        <v>171</v>
+      </c>
+      <c r="G4" s="35">
+        <v>48</v>
       </c>
       <c r="H4" s="26" t="s">
         <v>205</v>
@@ -2496,43 +2575,43 @@
       <c r="I4" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="J4" s="11" t="s">
-        <v>158</v>
+      <c r="J4" s="22" t="s">
+        <v>162</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>159</v>
-      </c>
-      <c r="L4" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="L4" s="53" t="s">
+        <v>280</v>
+      </c>
+      <c r="M4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N4" s="12" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" s="22" customFormat="1">
+    </row>
+    <row r="5" spans="1:15" s="22" customFormat="1">
       <c r="A5" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="B5" s="24">
-        <v>36</v>
+      <c r="B5" s="24" t="s">
+        <v>170</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="37" t="s">
         <v>60</v>
       </c>
       <c r="E5" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F5" s="18" t="s">
-        <v>188</v>
-      </c>
-      <c r="G5" s="40">
-        <v>45</v>
+      <c r="F5" s="21" t="s">
+        <v>172</v>
+      </c>
+      <c r="G5" s="35">
+        <v>48</v>
       </c>
       <c r="H5" s="26" t="s">
         <v>205</v>
@@ -2540,40 +2619,43 @@
       <c r="I5" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="J5" s="11" t="s">
-        <v>185</v>
-      </c>
-      <c r="K5" s="11" t="s">
-        <v>160</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="J5" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="L5" s="54" t="s">
+        <v>281</v>
+      </c>
+      <c r="M5" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M5" s="1" t="s">
+      <c r="N5" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="22" customFormat="1">
+    <row r="6" spans="1:15" s="22" customFormat="1">
       <c r="A6" s="22" t="s">
         <v>211</v>
       </c>
-      <c r="B6" s="24" t="s">
-        <v>164</v>
+      <c r="B6" s="13" t="s">
+        <v>157</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D6" s="37" t="s">
+      <c r="D6" s="34" t="s">
         <v>60</v>
       </c>
       <c r="E6" s="12" t="s">
         <v>60</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="G6" s="42">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="H6" s="26" t="s">
         <v>205</v>
@@ -2581,23 +2663,26 @@
       <c r="I6" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="J6" s="22" t="s">
-        <v>186</v>
-      </c>
-      <c r="K6" s="22" t="s">
-        <v>161</v>
-      </c>
-      <c r="L6" s="1" t="s">
+      <c r="J6" s="11" t="s">
+        <v>158</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>159</v>
+      </c>
+      <c r="L6" s="54" t="s">
+        <v>276</v>
+      </c>
+      <c r="M6" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="O6" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="22" customFormat="1">
+    <row r="7" spans="1:15" s="22" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>212</v>
       </c>
@@ -2631,37 +2716,40 @@
       <c r="K7" s="22" t="s">
         <v>163</v>
       </c>
-      <c r="L7" s="1" t="s">
+      <c r="L7" s="53" t="s">
+        <v>279</v>
+      </c>
+      <c r="M7" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="N7" s="12" t="s">
+      <c r="O7" s="12" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="22" customFormat="1">
+    <row r="8" spans="1:15" s="22" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>213</v>
       </c>
-      <c r="B8" s="24" t="s">
-        <v>167</v>
+      <c r="B8" s="24">
+        <v>36</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>259</v>
       </c>
-      <c r="D8" s="37" t="s">
+      <c r="D8" s="34" t="s">
         <v>60</v>
       </c>
       <c r="E8" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F8" s="21" t="s">
-        <v>171</v>
-      </c>
-      <c r="G8" s="35">
-        <v>48</v>
+      <c r="F8" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="40">
+        <v>45</v>
       </c>
       <c r="H8" s="26" t="s">
         <v>205</v>
@@ -2669,25 +2757,28 @@
       <c r="I8" s="26" t="s">
         <v>197</v>
       </c>
-      <c r="J8" s="22" t="s">
-        <v>162</v>
+      <c r="J8" s="11" t="s">
+        <v>185</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>168</v>
-      </c>
-      <c r="L8" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L8" s="53" t="s">
+        <v>277</v>
+      </c>
+      <c r="M8" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="22" customFormat="1">
+    <row r="9" spans="1:15" s="22" customFormat="1">
       <c r="A9" s="22" t="s">
         <v>214</v>
       </c>
       <c r="B9" s="24" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>259</v>
@@ -2699,10 +2790,10 @@
         <v>60</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>172</v>
-      </c>
-      <c r="G9" s="35">
-        <v>48</v>
+        <v>187</v>
+      </c>
+      <c r="G9" s="42">
+        <v>5</v>
       </c>
       <c r="H9" s="26" t="s">
         <v>205</v>
@@ -2711,19 +2802,25 @@
         <v>197</v>
       </c>
       <c r="J9" s="22" t="s">
-        <v>162</v>
+        <v>186</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>169</v>
-      </c>
-      <c r="L9" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="L9" s="53" t="s">
+        <v>278</v>
+      </c>
+      <c r="M9" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="10" spans="1:14" s="22" customFormat="1">
+      <c r="O9" s="12" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" s="22" customFormat="1">
       <c r="A10" s="22" t="s">
         <v>215</v>
       </c>
@@ -2757,14 +2854,17 @@
       <c r="K10" s="22" t="s">
         <v>174</v>
       </c>
-      <c r="L10" s="1" t="s">
+      <c r="L10" s="54" t="s">
+        <v>282</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="22" customFormat="1">
+    <row r="11" spans="1:15" s="22" customFormat="1">
       <c r="A11" s="22" t="s">
         <v>216</v>
       </c>
@@ -2798,15 +2898,18 @@
       <c r="K11" s="22" t="s">
         <v>175</v>
       </c>
-      <c r="L11" s="1" t="s">
+      <c r="L11" s="53" t="s">
+        <v>283</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="22" customFormat="1">
-      <c r="A12" s="22" t="s">
+    <row r="12" spans="1:15" s="22" customFormat="1">
+      <c r="A12" s="1" t="s">
         <v>217</v>
       </c>
       <c r="B12" s="20" t="s">
@@ -2837,14 +2940,15 @@
         <v>15</v>
       </c>
       <c r="K12" s="6"/>
-      <c r="L12" s="1" t="s">
+      <c r="L12" s="6"/>
+      <c r="M12" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="22" customFormat="1">
+    <row r="13" spans="1:15" s="22" customFormat="1">
       <c r="A13" s="22" t="s">
         <v>218</v>
       </c>
@@ -2878,14 +2982,15 @@
       <c r="K13" s="6" t="s">
         <v>67</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="6"/>
+      <c r="M13" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="22" customFormat="1">
+    <row r="14" spans="1:15" s="22" customFormat="1">
       <c r="A14" s="22" t="s">
         <v>219</v>
       </c>
@@ -2919,14 +3024,15 @@
       <c r="K14" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="L14" s="1" t="s">
+      <c r="L14" s="6"/>
+      <c r="M14" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="22" customFormat="1">
+    <row r="15" spans="1:15" s="22" customFormat="1">
       <c r="A15" s="22" t="s">
         <v>220</v>
       </c>
@@ -2960,17 +3066,18 @@
       <c r="K15" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="L15" s="1" t="s">
+      <c r="L15" s="6"/>
+      <c r="M15" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N15" s="22" t="s">
+      <c r="O15" s="22" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="22" customFormat="1">
+    <row r="16" spans="1:15" s="22" customFormat="1">
       <c r="A16" s="22" t="s">
         <v>221</v>
       </c>
@@ -3004,14 +3111,15 @@
       <c r="K16" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="6"/>
+      <c r="M16" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="17" spans="1:14" s="22" customFormat="1">
+    <row r="17" spans="1:15" s="22" customFormat="1">
       <c r="A17" s="22" t="s">
         <v>222</v>
       </c>
@@ -3045,17 +3153,18 @@
       <c r="K17" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="6"/>
+      <c r="M17" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N17" s="22" t="s">
+      <c r="O17" s="22" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="22" customFormat="1">
+    <row r="18" spans="1:15" s="22" customFormat="1">
       <c r="A18" s="22" t="s">
         <v>223</v>
       </c>
@@ -3089,14 +3198,15 @@
       <c r="K18" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="6"/>
+      <c r="M18" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="22" customFormat="1">
+    <row r="19" spans="1:15" s="22" customFormat="1">
       <c r="A19" s="22" t="s">
         <v>224</v>
       </c>
@@ -3130,17 +3240,18 @@
       <c r="K19" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="6"/>
+      <c r="M19" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N19" s="22" t="s">
+      <c r="O19" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="22" customFormat="1">
+    <row r="20" spans="1:15" s="22" customFormat="1">
       <c r="A20" s="22" t="s">
         <v>225</v>
       </c>
@@ -3174,14 +3285,15 @@
       <c r="K20" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="6"/>
+      <c r="M20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:14" s="22" customFormat="1">
+    <row r="21" spans="1:15" s="22" customFormat="1">
       <c r="A21" s="22" t="s">
         <v>226</v>
       </c>
@@ -3215,14 +3327,15 @@
       <c r="K21" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L21" s="6"/>
+      <c r="M21" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="22" customFormat="1">
+    <row r="22" spans="1:15" s="22" customFormat="1">
       <c r="A22" s="22" t="s">
         <v>227</v>
       </c>
@@ -3256,14 +3369,15 @@
       <c r="K22" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="L22" s="1" t="s">
+      <c r="L22" s="6"/>
+      <c r="M22" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:14" s="22" customFormat="1">
+    <row r="23" spans="1:15" s="22" customFormat="1">
       <c r="A23" s="22" t="s">
         <v>228</v>
       </c>
@@ -3297,17 +3411,18 @@
       <c r="K23" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="L23" s="1" t="s">
+      <c r="L23" s="6"/>
+      <c r="M23" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N23" s="22" t="s">
+      <c r="O23" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="22" customFormat="1">
+    <row r="24" spans="1:15" s="22" customFormat="1">
       <c r="A24" s="22" t="s">
         <v>229</v>
       </c>
@@ -3341,14 +3456,15 @@
       <c r="K24" s="6" t="s">
         <v>269</v>
       </c>
-      <c r="L24" s="1" t="s">
+      <c r="L24" s="6"/>
+      <c r="M24" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="22" customFormat="1">
+    <row r="25" spans="1:15" s="22" customFormat="1">
       <c r="A25" s="22" t="s">
         <v>230</v>
       </c>
@@ -3382,14 +3498,15 @@
       <c r="K25" s="6" t="s">
         <v>255</v>
       </c>
-      <c r="L25" s="1" t="s">
+      <c r="L25" s="6"/>
+      <c r="M25" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M25" s="1" t="s">
+      <c r="N25" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="22" customFormat="1">
+    <row r="26" spans="1:15" s="22" customFormat="1">
       <c r="A26" s="16" t="s">
         <v>231</v>
       </c>
@@ -3421,17 +3538,18 @@
         <v>41</v>
       </c>
       <c r="K26" s="9"/>
-      <c r="L26" s="2" t="s">
+      <c r="L26" s="9"/>
+      <c r="M26" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="M26" s="2" t="s">
+      <c r="N26" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="N26" s="16" t="s">
+      <c r="O26" s="16" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="22" customFormat="1">
+    <row r="27" spans="1:15" s="22" customFormat="1">
       <c r="A27" s="22" t="s">
         <v>232</v>
       </c>
@@ -3465,14 +3583,15 @@
       <c r="K27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="L27" s="6"/>
+      <c r="M27" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="N27" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="22" customFormat="1">
+    <row r="28" spans="1:15" s="22" customFormat="1">
       <c r="A28" s="22" t="s">
         <v>233</v>
       </c>
@@ -3504,17 +3623,18 @@
         <v>46</v>
       </c>
       <c r="K28" s="6"/>
-      <c r="L28" s="12" t="s">
+      <c r="L28" s="6"/>
+      <c r="M28" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="N28" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N28" s="22" t="s">
+      <c r="O28" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="22" customFormat="1">
+    <row r="29" spans="1:15" s="22" customFormat="1">
       <c r="A29" s="22" t="s">
         <v>234</v>
       </c>
@@ -3548,14 +3668,15 @@
       <c r="K29" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="L29" s="12" t="s">
+      <c r="L29" s="6"/>
+      <c r="M29" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M29" s="1" t="s">
+      <c r="N29" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="22" customFormat="1">
+    <row r="30" spans="1:15" s="22" customFormat="1">
       <c r="A30" s="22" t="s">
         <v>235</v>
       </c>
@@ -3589,14 +3710,15 @@
       <c r="K30" s="6" t="s">
         <v>97</v>
       </c>
-      <c r="L30" s="12" t="s">
+      <c r="L30" s="6"/>
+      <c r="M30" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M30" s="1" t="s">
+      <c r="N30" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="22" customFormat="1">
+    <row r="31" spans="1:15" s="22" customFormat="1">
       <c r="A31" s="22" t="s">
         <v>236</v>
       </c>
@@ -3630,14 +3752,15 @@
       <c r="K31" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="L31" s="12" t="s">
+      <c r="L31" s="6"/>
+      <c r="M31" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M31" s="1" t="s">
+      <c r="N31" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="22" customFormat="1">
+    <row r="32" spans="1:15" s="22" customFormat="1">
       <c r="A32" s="22" t="s">
         <v>237</v>
       </c>
@@ -3669,14 +3792,15 @@
         <v>49</v>
       </c>
       <c r="K32" s="6"/>
-      <c r="L32" s="12" t="s">
+      <c r="L32" s="6"/>
+      <c r="M32" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M32" s="1" t="s">
+      <c r="N32" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="22" customFormat="1">
+    <row r="33" spans="1:15" s="22" customFormat="1">
       <c r="A33" s="22" t="s">
         <v>238</v>
       </c>
@@ -3710,14 +3834,15 @@
       <c r="K33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="L33" s="12" t="s">
+      <c r="L33" s="6"/>
+      <c r="M33" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M33" s="1" t="s">
+      <c r="N33" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="22" customFormat="1">
+    <row r="34" spans="1:15" s="22" customFormat="1">
       <c r="A34" s="22" t="s">
         <v>239</v>
       </c>
@@ -3749,14 +3874,15 @@
         <v>3</v>
       </c>
       <c r="K34" s="6"/>
-      <c r="L34" s="12" t="s">
+      <c r="L34" s="6"/>
+      <c r="M34" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M34" s="1" t="s">
+      <c r="N34" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="22" customFormat="1">
+    <row r="35" spans="1:15" s="22" customFormat="1">
       <c r="A35" s="22" t="s">
         <v>240</v>
       </c>
@@ -3790,14 +3916,15 @@
       <c r="K35" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="L35" s="12" t="s">
+      <c r="L35" s="6"/>
+      <c r="M35" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M35" s="1" t="s">
+      <c r="N35" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="22" customFormat="1">
+    <row r="36" spans="1:15" s="22" customFormat="1">
       <c r="A36" s="22" t="s">
         <v>241</v>
       </c>
@@ -3829,14 +3956,15 @@
         <v>37</v>
       </c>
       <c r="K36" s="6"/>
-      <c r="L36" s="12" t="s">
+      <c r="L36" s="6"/>
+      <c r="M36" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M36" s="1" t="s">
+      <c r="N36" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="22" customFormat="1">
+    <row r="37" spans="1:15" s="22" customFormat="1">
       <c r="A37" s="22" t="s">
         <v>242</v>
       </c>
@@ -3868,14 +3996,15 @@
         <v>9</v>
       </c>
       <c r="K37" s="6"/>
-      <c r="L37" s="12" t="s">
+      <c r="L37" s="6"/>
+      <c r="M37" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M37" s="1" t="s">
+      <c r="N37" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="22" customFormat="1">
+    <row r="38" spans="1:15" s="22" customFormat="1">
       <c r="A38" s="22" t="s">
         <v>243</v>
       </c>
@@ -3907,14 +4036,15 @@
         <v>11</v>
       </c>
       <c r="K38" s="6"/>
-      <c r="L38" s="12" t="s">
+      <c r="L38" s="6"/>
+      <c r="M38" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M38" s="1" t="s">
+      <c r="N38" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:14" s="22" customFormat="1">
+    <row r="39" spans="1:15" s="22" customFormat="1">
       <c r="A39" s="22" t="s">
         <v>244</v>
       </c>
@@ -3948,17 +4078,18 @@
       <c r="K39" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="L39" s="12" t="s">
+      <c r="L39" s="6"/>
+      <c r="M39" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M39" s="1" t="s">
+      <c r="N39" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N39" s="22" t="s">
+      <c r="O39" s="22" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="40" spans="1:14" s="22" customFormat="1">
+    <row r="40" spans="1:15" s="22" customFormat="1">
       <c r="A40" s="22" t="s">
         <v>245</v>
       </c>
@@ -3992,14 +4123,14 @@
       <c r="K40" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="L40" s="12" t="s">
+      <c r="M40" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M40" s="1" t="s">
+      <c r="N40" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="41" spans="1:14" s="22" customFormat="1">
+    <row r="41" spans="1:15" s="22" customFormat="1">
       <c r="A41" s="22" t="s">
         <v>246</v>
       </c>
@@ -4033,14 +4164,15 @@
       <c r="K41" s="12" t="s">
         <v>124</v>
       </c>
-      <c r="L41" s="12" t="s">
+      <c r="L41" s="12"/>
+      <c r="M41" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M41" s="1" t="s">
+      <c r="N41" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="42" spans="1:14" s="22" customFormat="1">
+    <row r="42" spans="1:15" s="22" customFormat="1">
       <c r="A42" s="22" t="s">
         <v>247</v>
       </c>
@@ -4074,14 +4206,15 @@
       <c r="K42" s="11" t="s">
         <v>127</v>
       </c>
-      <c r="L42" s="12" t="s">
+      <c r="L42" s="11"/>
+      <c r="M42" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M42" s="1" t="s">
+      <c r="N42" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="43" spans="1:14" s="22" customFormat="1">
+    <row r="43" spans="1:15" s="22" customFormat="1">
       <c r="A43" s="22" t="s">
         <v>260</v>
       </c>
@@ -4115,17 +4248,17 @@
       <c r="K43" s="22" t="s">
         <v>137</v>
       </c>
-      <c r="L43" s="12" t="s">
+      <c r="M43" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M43" s="1" t="s">
+      <c r="N43" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N43" s="11" t="s">
+      <c r="O43" s="11" t="s">
         <v>194</v>
       </c>
     </row>
-    <row r="44" spans="1:14" s="22" customFormat="1">
+    <row r="44" spans="1:15" s="22" customFormat="1">
       <c r="A44" s="22" t="s">
         <v>261</v>
       </c>
@@ -4157,17 +4290,18 @@
         <v>54</v>
       </c>
       <c r="K44" s="6"/>
-      <c r="L44" s="12" t="s">
+      <c r="L44" s="6"/>
+      <c r="M44" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M44" s="1" t="s">
+      <c r="N44" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="N44" s="22" t="s">
+      <c r="O44" s="22" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="45" spans="1:14" s="22" customFormat="1">
+    <row r="45" spans="1:15" s="22" customFormat="1">
       <c r="A45" s="22" t="s">
         <v>262</v>
       </c>
@@ -4201,14 +4335,15 @@
       <c r="K45" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="L45" s="12" t="s">
+      <c r="L45" s="6"/>
+      <c r="M45" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M45" s="1" t="s">
+      <c r="N45" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="46" spans="1:14" s="22" customFormat="1">
+    <row r="46" spans="1:15" s="22" customFormat="1">
       <c r="A46" s="22" t="s">
         <v>263</v>
       </c>
@@ -4242,14 +4377,15 @@
       <c r="K46" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="L46" s="12" t="s">
+      <c r="L46" s="6"/>
+      <c r="M46" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M46" s="1" t="s">
+      <c r="N46" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="47" spans="1:14" s="22" customFormat="1">
+    <row r="47" spans="1:15" s="22" customFormat="1">
       <c r="A47" s="22" t="s">
         <v>264</v>
       </c>
@@ -4283,14 +4419,15 @@
       <c r="K47" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="L47" s="12" t="s">
+      <c r="L47" s="6"/>
+      <c r="M47" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="M47" s="1" t="s">
+      <c r="N47" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="48" spans="1:14" s="22" customFormat="1">
+    <row r="48" spans="1:15" s="22" customFormat="1">
       <c r="A48" s="16" t="s">
         <v>265</v>
       </c>
@@ -4322,17 +4459,18 @@
         <v>57</v>
       </c>
       <c r="K48" s="9"/>
-      <c r="L48" s="15" t="s">
+      <c r="L48" s="9"/>
+      <c r="M48" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="M48" s="2" t="s">
+      <c r="N48" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="N48" s="16"/>
+      <c r="O48" s="16"/>
     </row>
   </sheetData>
-  <sortState ref="A2:P48">
-    <sortCondition ref="A2:A48"/>
+  <sortState ref="A2:O11">
+    <sortCondition ref="A2:A11"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>